<commit_message>
BUGFIX: append sentinel to unsearchable stocks
</commit_message>
<xml_diff>
--- a/StockScreener - Copy.xlsx
+++ b/StockScreener - Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathan\PycharmProjects\StockScreener\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1C883F-1ACA-4176-AD8E-A5C6D3CBBA1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29DC94D-B805-4965-AF29-DEEAF97B07CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="4680" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="companylist" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">companylist!$A$2:$A$9929</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31412,8 +31412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L10170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3644" workbookViewId="0">
-      <selection activeCell="F3660" sqref="F3660"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
BUGFIX: fix indexing issue of stocks
</commit_message>
<xml_diff>
--- a/StockScreener - Copy.xlsx
+++ b/StockScreener - Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathan\PycharmProjects\StockScreener\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29DC94D-B805-4965-AF29-DEEAF97B07CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CBCAAE4-E7DC-4E6C-86F4-8ACD1BC3A08F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="6165" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="companylist" sheetId="1" r:id="rId1"/>
@@ -31412,8 +31412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L10170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A10116" workbookViewId="0">
+      <selection activeCell="H10120" sqref="H10120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Ks add calculations (#5)
* Added Priority, stock interpretter, testing for best returns depending on priorities. Added extra filters for screener. Changed file naming scheme

* Added Stock interpretter

* Removed fixed multiplier

* BUGFIX: fix indexing issue of stocks
</commit_message>
<xml_diff>
--- a/StockScreener - Copy.xlsx
+++ b/StockScreener - Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathan\PycharmProjects\StockScreener\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29DC94D-B805-4965-AF29-DEEAF97B07CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CBCAAE4-E7DC-4E6C-86F4-8ACD1BC3A08F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="6165" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="companylist" sheetId="1" r:id="rId1"/>
@@ -31412,8 +31412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L10170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A10116" workbookViewId="0">
+      <selection activeCell="H10120" sqref="H10120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>